<commit_message>
Fix using of pd.period_range() replacing it for pd.date_range().
</commit_message>
<xml_diff>
--- a/xlseries/tests/integration_cases/expected/test_case2.xlsx
+++ b/xlseries/tests/integration_cases/expected/test_case2.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -1423,9 +1423,1651 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV147"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="14.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="5" customWidth="1"/>
+    <col min="3" max="256" width="8.125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" customHeight="1">
+      <c r="A2" s="7">
+        <v>37316</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2.398855555555556</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" customHeight="1">
+      <c r="A3" s="7">
+        <v>37347</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.8551062500000008</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="17" customHeight="1">
+      <c r="A4" s="7">
+        <v>37377</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.3287</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="17" customHeight="1">
+      <c r="A5" s="7">
+        <v>37408</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3.621300000000002</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="17" customHeight="1">
+      <c r="A6" s="7">
+        <v>37438</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3.6071363636363638</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="17" customHeight="1">
+      <c r="A7" s="7">
+        <v>37469</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3.6207095238095239</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="17" customHeight="1">
+      <c r="A8" s="7">
+        <v>37500</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3.6430761904761901</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" customHeight="1">
+      <c r="A9" s="7">
+        <v>37530</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3.6518818181818191</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="17" customHeight="1">
+      <c r="A10" s="7">
+        <v>37561</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3.52555</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" customHeight="1">
+      <c r="A11" s="7">
+        <v>37591</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3.4901714285714278</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="17" customHeight="1">
+      <c r="A12" s="7">
+        <v>37622</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3.258186363636363</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="17" customHeight="1">
+      <c r="A13" s="7">
+        <v>37653</v>
+      </c>
+      <c r="B13" s="8">
+        <v>3.1631649999999989</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="17" customHeight="1">
+      <c r="A14" s="7">
+        <v>37681</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3.0747249999999999</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="17" customHeight="1">
+      <c r="A15" s="7">
+        <v>37712</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2.8946049999999999</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="17" customHeight="1">
+      <c r="A16" s="7">
+        <v>37742</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2.8356714285714291</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="17" customHeight="1">
+      <c r="A17" s="7">
+        <v>37773</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2.8088500000000001</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="17" customHeight="1">
+      <c r="A18" s="7">
+        <v>37803</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2.801286363636363</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" customHeight="1">
+      <c r="A19" s="7">
+        <v>37834</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2.92849</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="17" customHeight="1">
+      <c r="A20" s="7">
+        <v>37865</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2.9209454545454552</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="17" customHeight="1">
+      <c r="A21" s="7">
+        <v>37895</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2.859049999999999</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="17" customHeight="1">
+      <c r="A22" s="7">
+        <v>37926</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2.8839210526315791</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="17" customHeight="1">
+      <c r="A23" s="7">
+        <v>37956</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2.9606238095238089</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="17" customHeight="1">
+      <c r="A24" s="7">
+        <v>37987</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2.892842857142857</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="17" customHeight="1">
+      <c r="A25" s="7">
+        <v>38018</v>
+      </c>
+      <c r="B25" s="8">
+        <v>2.9319199999999999</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" customHeight="1">
+      <c r="A26" s="7">
+        <v>38047</v>
+      </c>
+      <c r="B26" s="8">
+        <v>2.8975652173913051</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="17" customHeight="1">
+      <c r="A27" s="7">
+        <v>38078</v>
+      </c>
+      <c r="B27" s="8">
+        <v>2.8359157894736842</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="17" customHeight="1">
+      <c r="A28" s="7">
+        <v>38108</v>
+      </c>
+      <c r="B28" s="8">
+        <v>2.9196750000000011</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="17" customHeight="1">
+      <c r="A29" s="7">
+        <v>38139</v>
+      </c>
+      <c r="B29" s="8">
+        <v>2.9602571428571429</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="17" customHeight="1">
+      <c r="A30" s="7">
+        <v>38169</v>
+      </c>
+      <c r="B30" s="8">
+        <v>2.9552142857142849</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="17" customHeight="1">
+      <c r="A31" s="7">
+        <v>38200</v>
+      </c>
+      <c r="B31" s="8">
+        <v>3.013580952380952</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="17" customHeight="1">
+      <c r="A32" s="7">
+        <v>38231</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2.996013636363636</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="17" customHeight="1">
+      <c r="A33" s="7">
+        <v>38261</v>
+      </c>
+      <c r="B33" s="8">
+        <v>2.9691800000000002</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="17" customHeight="1">
+      <c r="A34" s="7">
+        <v>38292</v>
+      </c>
+      <c r="B34" s="8">
+        <v>2.9546363636363639</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="17" customHeight="1">
+      <c r="A35" s="7">
+        <v>38322</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2.970918181818182</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="17" customHeight="1">
+      <c r="A36" s="7">
+        <v>38353</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2.9460285714285721</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" ht="17" customHeight="1">
+      <c r="A37" s="7">
+        <v>38384</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2.915344999999999</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" ht="17" customHeight="1">
+      <c r="A38" s="7">
+        <v>38412</v>
+      </c>
+      <c r="B38" s="8">
+        <v>2.9265523809523808</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="17" customHeight="1">
+      <c r="A39" s="7">
+        <v>38443</v>
+      </c>
+      <c r="B39" s="8">
+        <v>2.9004142857142861</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="17" customHeight="1">
+      <c r="A40" s="7">
+        <v>38473</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2.89094761904762</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" ht="17" customHeight="1">
+      <c r="A41" s="7">
+        <v>38504</v>
+      </c>
+      <c r="B41" s="8">
+        <v>2.8835904761904758</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" ht="17" customHeight="1">
+      <c r="A42" s="7">
+        <v>38534</v>
+      </c>
+      <c r="B42" s="8">
+        <v>2.869566666666667</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" ht="17" customHeight="1">
+      <c r="A43" s="7">
+        <v>38565</v>
+      </c>
+      <c r="B43" s="8">
+        <v>2.888018181818182</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="17" customHeight="1">
+      <c r="A44" s="7">
+        <v>38596</v>
+      </c>
+      <c r="B44" s="8">
+        <v>2.9117136363636358</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" ht="17" customHeight="1">
+      <c r="A45" s="7">
+        <v>38626</v>
+      </c>
+      <c r="B45" s="8">
+        <v>2.9660449999999998</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="17" customHeight="1">
+      <c r="A46" s="7">
+        <v>38657</v>
+      </c>
+      <c r="B46" s="8">
+        <v>2.9672181818181809</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="17" customHeight="1">
+      <c r="A47" s="7">
+        <v>38687</v>
+      </c>
+      <c r="B47" s="8">
+        <v>3.0144523809523811</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" ht="17" customHeight="1">
+      <c r="A48" s="7">
+        <v>38718</v>
+      </c>
+      <c r="B48" s="8">
+        <v>3.0460363636363641</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" ht="17" customHeight="1">
+      <c r="A49" s="7">
+        <v>38749</v>
+      </c>
+      <c r="B49" s="8">
+        <v>3.068905</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="17" customHeight="1">
+      <c r="A50" s="7">
+        <v>38777</v>
+      </c>
+      <c r="B50" s="8">
+        <v>3.0763272727272728</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" ht="17" customHeight="1">
+      <c r="A51" s="7">
+        <v>38808</v>
+      </c>
+      <c r="B51" s="8">
+        <v>3.0662666666666669</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5" ht="17" customHeight="1">
+      <c r="A52" s="7">
+        <v>38838</v>
+      </c>
+      <c r="B52" s="8">
+        <v>3.0534809523809519</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5" ht="17" customHeight="1">
+      <c r="A53" s="7">
+        <v>38869</v>
+      </c>
+      <c r="B53" s="8">
+        <v>3.0812666666666662</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5" ht="17" customHeight="1">
+      <c r="A54" s="7">
+        <v>38899</v>
+      </c>
+      <c r="B54" s="8">
+        <v>3.0819619047619051</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:5" ht="17" customHeight="1">
+      <c r="A55" s="7">
+        <v>38930</v>
+      </c>
+      <c r="B55" s="8">
+        <v>3.0789727272727272</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:5" ht="17" customHeight="1">
+      <c r="A56" s="7">
+        <v>38961</v>
+      </c>
+      <c r="B56" s="8">
+        <v>3.1000714285714279</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5" ht="17" customHeight="1">
+      <c r="A57" s="7">
+        <v>38991</v>
+      </c>
+      <c r="B57" s="8">
+        <v>3.0984761904761902</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5" ht="17" customHeight="1">
+      <c r="A58" s="7">
+        <v>39022</v>
+      </c>
+      <c r="B58" s="8">
+        <v>3.075738095238095</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5" ht="17" customHeight="1">
+      <c r="A59" s="7">
+        <v>39052</v>
+      </c>
+      <c r="B59" s="8">
+        <v>3.0602684210526312</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:5" ht="17" customHeight="1">
+      <c r="A60" s="7">
+        <v>39083</v>
+      </c>
+      <c r="B60" s="8">
+        <v>3.085040909090909</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:5" ht="17" customHeight="1">
+      <c r="A61" s="7">
+        <v>39114</v>
+      </c>
+      <c r="B61" s="8">
+        <v>3.1026250000000002</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:5" ht="17" customHeight="1">
+      <c r="A62" s="7">
+        <v>39142</v>
+      </c>
+      <c r="B62" s="8">
+        <v>3.101040909090909</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="1:5" ht="17" customHeight="1">
+      <c r="A63" s="7">
+        <v>39173</v>
+      </c>
+      <c r="B63" s="8">
+        <v>3.089055555555555</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:5" ht="17" customHeight="1">
+      <c r="A64" s="7">
+        <v>39203</v>
+      </c>
+      <c r="B64" s="8">
+        <v>3.0800142857142871</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:5" ht="17" customHeight="1">
+      <c r="A65" s="7">
+        <v>39234</v>
+      </c>
+      <c r="B65" s="8">
+        <v>3.0792649999999999</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="1:5" ht="17" customHeight="1">
+      <c r="A66" s="7">
+        <v>39264</v>
+      </c>
+      <c r="B66" s="8">
+        <v>3.1116285714285721</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:5" ht="17" customHeight="1">
+      <c r="A67" s="7">
+        <v>39295</v>
+      </c>
+      <c r="B67" s="8">
+        <v>3.1523590909090902</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:5" ht="17" customHeight="1">
+      <c r="A68" s="7">
+        <v>39326</v>
+      </c>
+      <c r="B68" s="8">
+        <v>3.1474549999999999</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:5" ht="17" customHeight="1">
+      <c r="A69" s="7">
+        <v>39356</v>
+      </c>
+      <c r="B69" s="8">
+        <v>3.1604454545454539</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:5" ht="17" customHeight="1">
+      <c r="A70" s="7">
+        <v>39387</v>
+      </c>
+      <c r="B70" s="8">
+        <v>3.1359142857142861</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" ht="17" customHeight="1">
+      <c r="A71" s="7">
+        <v>39417</v>
+      </c>
+      <c r="B71" s="8">
+        <v>3.1396500000000001</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="1:5" ht="17" customHeight="1">
+      <c r="A72" s="7">
+        <v>39448</v>
+      </c>
+      <c r="B72" s="8">
+        <v>3.1444181818181818</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="1:5" ht="17" customHeight="1">
+      <c r="A73" s="7">
+        <v>39479</v>
+      </c>
+      <c r="B73" s="8">
+        <v>3.1583142857142859</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="1:5" ht="17" customHeight="1">
+      <c r="A74" s="7">
+        <v>39508</v>
+      </c>
+      <c r="B74" s="8">
+        <v>3.1558388888888889</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="1:5" ht="17" customHeight="1">
+      <c r="A75" s="7">
+        <v>39539</v>
+      </c>
+      <c r="B75" s="8">
+        <v>3.1665428571428582</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="1:5" ht="17" customHeight="1">
+      <c r="A76" s="7">
+        <v>39569</v>
+      </c>
+      <c r="B76" s="8">
+        <v>3.1511</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:5" ht="17" customHeight="1">
+      <c r="A77" s="7">
+        <v>39600</v>
+      </c>
+      <c r="B77" s="8">
+        <v>3.0433500000000011</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="1:5" ht="17" customHeight="1">
+      <c r="A78" s="7">
+        <v>39630</v>
+      </c>
+      <c r="B78" s="8">
+        <v>3.0223454545454551</v>
+      </c>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="1:5" ht="17" customHeight="1">
+      <c r="A79" s="7">
+        <v>39661</v>
+      </c>
+      <c r="B79" s="8">
+        <v>3.0332750000000002</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="1:5" ht="17" customHeight="1">
+      <c r="A80" s="7">
+        <v>39692</v>
+      </c>
+      <c r="B80" s="8">
+        <v>3.0823636363636369</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5" ht="17" customHeight="1">
+      <c r="A81" s="7">
+        <v>39722</v>
+      </c>
+      <c r="B81" s="8">
+        <v>3.2385227272727271</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" customHeight="1">
+      <c r="A82" s="7">
+        <v>39753</v>
+      </c>
+      <c r="B82" s="8">
+        <v>3.329173684210526</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="1:5" ht="17" customHeight="1">
+      <c r="A83" s="7">
+        <v>39783</v>
+      </c>
+      <c r="B83" s="8">
+        <v>3.4226333333333332</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="1:5" ht="17" customHeight="1">
+      <c r="A84" s="7">
+        <v>39814</v>
+      </c>
+      <c r="B84" s="8">
+        <v>3.4640142857142862</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="1:5" ht="17" customHeight="1">
+      <c r="A85" s="7">
+        <v>39845</v>
+      </c>
+      <c r="B85" s="8">
+        <v>3.5115149999999988</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="1:5" ht="17" customHeight="1">
+      <c r="A86" s="7">
+        <v>39873</v>
+      </c>
+      <c r="B86" s="8">
+        <v>3.6539714285714289</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="1:5" ht="17" customHeight="1">
+      <c r="A87" s="7">
+        <v>39904</v>
+      </c>
+      <c r="B87" s="8">
+        <v>3.6933736842105271</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="1:5" ht="17" customHeight="1">
+      <c r="A88" s="7">
+        <v>39934</v>
+      </c>
+      <c r="B88" s="8">
+        <v>3.7244736842105262</v>
+      </c>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="1:5" ht="17" customHeight="1">
+      <c r="A89" s="7">
+        <v>39965</v>
+      </c>
+      <c r="B89" s="8">
+        <v>3.7681333333333331</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="1:5" ht="17" customHeight="1">
+      <c r="A90" s="7">
+        <v>39995</v>
+      </c>
+      <c r="B90" s="8">
+        <v>3.809733333333333</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+    </row>
+    <row r="91" spans="1:5" ht="17" customHeight="1">
+      <c r="A91" s="7">
+        <v>40026</v>
+      </c>
+      <c r="B91" s="8">
+        <v>3.839175</v>
+      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="1:5" ht="17" customHeight="1">
+      <c r="A92" s="7">
+        <v>40057</v>
+      </c>
+      <c r="B92" s="8">
+        <v>3.842368181818181</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="1:5" ht="17" customHeight="1">
+      <c r="A93" s="7">
+        <v>40087</v>
+      </c>
+      <c r="B93" s="8">
+        <v>3.8262095238095242</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+    </row>
+    <row r="94" spans="1:5" ht="17" customHeight="1">
+      <c r="A94" s="7">
+        <v>40118</v>
+      </c>
+      <c r="B94" s="8">
+        <v>3.8109500000000001</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="1:5" ht="17" customHeight="1">
+      <c r="A95" s="7">
+        <v>40148</v>
+      </c>
+      <c r="B95" s="8">
+        <v>3.8070190476190482</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+    </row>
+    <row r="96" spans="1:5" ht="17" customHeight="1">
+      <c r="A96" s="7">
+        <v>40179</v>
+      </c>
+      <c r="B96" s="8">
+        <v>3.80416</v>
+      </c>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="1:5" ht="17" customHeight="1">
+      <c r="A97" s="7">
+        <v>40210</v>
+      </c>
+      <c r="B97" s="8">
+        <v>3.851235</v>
+      </c>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+    </row>
+    <row r="98" spans="1:5" ht="17" customHeight="1">
+      <c r="A98" s="7">
+        <v>40238</v>
+      </c>
+      <c r="B98" s="8">
+        <v>3.8627409090909088</v>
+      </c>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="1:5" ht="17" customHeight="1">
+      <c r="A99" s="7">
+        <v>40269</v>
+      </c>
+      <c r="B99" s="8">
+        <v>3.8760699999999999</v>
+      </c>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="1:5" ht="17" customHeight="1">
+      <c r="A100" s="7">
+        <v>40299</v>
+      </c>
+      <c r="B100" s="8">
+        <v>3.9019736842105259</v>
+      </c>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="1:5" ht="17" customHeight="1">
+      <c r="A101" s="7">
+        <v>40330</v>
+      </c>
+      <c r="B101" s="8">
+        <v>3.9265238095238102</v>
+      </c>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+    </row>
+    <row r="102" spans="1:5" ht="17" customHeight="1">
+      <c r="A102" s="7">
+        <v>40360</v>
+      </c>
+      <c r="B102" s="8">
+        <v>3.9348238095238099</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+    </row>
+    <row r="103" spans="1:5" ht="17" customHeight="1">
+      <c r="A103" s="7">
+        <v>40391</v>
+      </c>
+      <c r="B103" s="8">
+        <v>3.937609523809523</v>
+      </c>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="1:5" ht="17" customHeight="1">
+      <c r="A104" s="7">
+        <v>40422</v>
+      </c>
+      <c r="B104" s="8">
+        <v>3.9518909090909098</v>
+      </c>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="1:5" ht="17" customHeight="1">
+      <c r="A105" s="7">
+        <v>40452</v>
+      </c>
+      <c r="B105" s="8">
+        <v>3.9569999999999999</v>
+      </c>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+    </row>
+    <row r="106" spans="1:5" ht="17" customHeight="1">
+      <c r="A106" s="7">
+        <v>40483</v>
+      </c>
+      <c r="B106" s="8">
+        <v>3.9676</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="1:5" ht="17" customHeight="1">
+      <c r="A107" s="7">
+        <v>40513</v>
+      </c>
+      <c r="B107" s="8">
+        <v>3.9776250000000002</v>
+      </c>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+    </row>
+    <row r="108" spans="1:5" ht="17" customHeight="1">
+      <c r="A108" s="7">
+        <v>40544</v>
+      </c>
+      <c r="B108" s="8">
+        <v>3.9813000000000001</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="1:5" ht="17" customHeight="1">
+      <c r="A109" s="7">
+        <v>40575</v>
+      </c>
+      <c r="B109" s="8">
+        <v>4.0220000000000002</v>
+      </c>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" spans="1:5" ht="17" customHeight="1">
+      <c r="A110" s="7">
+        <v>40603</v>
+      </c>
+      <c r="B110" s="8">
+        <v>4.0372000000000003</v>
+      </c>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+    </row>
+    <row r="111" spans="1:5" ht="17" customHeight="1">
+      <c r="A111" s="7">
+        <v>40634</v>
+      </c>
+      <c r="B111" s="8">
+        <v>4.0655000000000001</v>
+      </c>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+    </row>
+    <row r="112" spans="1:5" ht="17" customHeight="1">
+      <c r="A112" s="7">
+        <v>40664</v>
+      </c>
+      <c r="B112" s="8">
+        <v>4.0838999999999999</v>
+      </c>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+    </row>
+    <row r="113" spans="1:5" ht="17" customHeight="1">
+      <c r="A113" s="7">
+        <v>40695</v>
+      </c>
+      <c r="B113" s="8">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+    </row>
+    <row r="114" spans="1:5" ht="17" customHeight="1">
+      <c r="A114" s="7">
+        <v>40725</v>
+      </c>
+      <c r="B114" s="8">
+        <v>4.1276000000000002</v>
+      </c>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+    </row>
+    <row r="115" spans="1:5" ht="17" customHeight="1">
+      <c r="A115" s="7">
+        <v>40756</v>
+      </c>
+      <c r="B115" s="8">
+        <v>4.1680000000000001</v>
+      </c>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="1:5" ht="17" customHeight="1">
+      <c r="A116" s="7">
+        <v>40787</v>
+      </c>
+      <c r="B116" s="8">
+        <v>4.2042000000000002</v>
+      </c>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="1:5" ht="17" customHeight="1">
+      <c r="A117" s="7">
+        <v>40817</v>
+      </c>
+      <c r="B117" s="8">
+        <v>4.2221249999999992</v>
+      </c>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="1:5" ht="17" customHeight="1">
+      <c r="A118" s="7">
+        <v>40848</v>
+      </c>
+      <c r="B118" s="8">
+        <v>4.2601142857142849</v>
+      </c>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="1:5" ht="17" customHeight="1">
+      <c r="A119" s="7">
+        <v>40878</v>
+      </c>
+      <c r="B119" s="8">
+        <v>4.2887894736842096</v>
+      </c>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="1:5" ht="17" customHeight="1">
+      <c r="A120" s="7">
+        <v>40909</v>
+      </c>
+      <c r="B120" s="8">
+        <v>4.3206238095238101</v>
+      </c>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="1:5" ht="17" customHeight="1">
+      <c r="A121" s="7">
+        <v>40940</v>
+      </c>
+      <c r="B121" s="8">
+        <v>4.3462944444444442</v>
+      </c>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="1:5" ht="17" customHeight="1">
+      <c r="A122" s="7">
+        <v>40969</v>
+      </c>
+      <c r="B122" s="8">
+        <v>4.3563136363636357</v>
+      </c>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+    </row>
+    <row r="123" spans="1:5" ht="17" customHeight="1">
+      <c r="A123" s="7">
+        <v>41000</v>
+      </c>
+      <c r="B123" s="8">
+        <v>4.3978000000000002</v>
+      </c>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="1:5" ht="17" customHeight="1">
+      <c r="A124" s="7">
+        <v>41030</v>
+      </c>
+      <c r="B124" s="8">
+        <v>4.4503761904761907</v>
+      </c>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+    </row>
+    <row r="125" spans="1:5" ht="17" customHeight="1">
+      <c r="A125" s="7">
+        <v>41061</v>
+      </c>
+      <c r="B125" s="8">
+        <v>4.4977549999999997</v>
+      </c>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+    </row>
+    <row r="126" spans="1:5" ht="17" customHeight="1">
+      <c r="A126" s="7">
+        <v>41091</v>
+      </c>
+      <c r="B126" s="8">
+        <v>4.5528095238095254</v>
+      </c>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="1:5" ht="17" customHeight="1">
+      <c r="A127" s="7">
+        <v>41122</v>
+      </c>
+      <c r="B127" s="8">
+        <v>4.6098272727272729</v>
+      </c>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="1:5" ht="17" customHeight="1">
+      <c r="A128" s="7">
+        <v>41153</v>
+      </c>
+      <c r="B128" s="8">
+        <v>4.6698947368421049</v>
+      </c>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+    </row>
+    <row r="129" spans="1:5" ht="17" customHeight="1">
+      <c r="A129" s="7">
+        <v>41183</v>
+      </c>
+      <c r="B129" s="8">
+        <v>4.7298500000000008</v>
+      </c>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
+      <c r="E129" s="6"/>
+    </row>
+    <row r="130" spans="1:5" ht="17" customHeight="1">
+      <c r="A130" s="7">
+        <v>41214</v>
+      </c>
+      <c r="B130" s="8">
+        <v>4.7973899999999992</v>
+      </c>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+    </row>
+    <row r="131" spans="1:5" ht="17" customHeight="1">
+      <c r="A131" s="7">
+        <v>41244</v>
+      </c>
+      <c r="B131" s="8">
+        <v>4.88</v>
+      </c>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+    </row>
+    <row r="132" spans="1:5" ht="17" customHeight="1">
+      <c r="A132" s="7">
+        <v>41275</v>
+      </c>
+      <c r="B132" s="8">
+        <v>4.9485999999999999</v>
+      </c>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="6"/>
+    </row>
+    <row r="133" spans="1:5" ht="17" customHeight="1">
+      <c r="A133" s="7">
+        <v>41306</v>
+      </c>
+      <c r="B133" s="8">
+        <v>5.0110999999999999</v>
+      </c>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+    </row>
+    <row r="134" spans="1:5" ht="17" customHeight="1">
+      <c r="A134" s="7">
+        <v>41334</v>
+      </c>
+      <c r="B134" s="8">
+        <v>5.0839999999999996</v>
+      </c>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+    </row>
+    <row r="135" spans="1:5" ht="17" customHeight="1">
+      <c r="A135" s="7">
+        <v>41365</v>
+      </c>
+      <c r="B135" s="8">
+        <v>5.1555</v>
+      </c>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+    </row>
+    <row r="136" spans="1:5" ht="17" customHeight="1">
+      <c r="A136" s="7">
+        <v>41395</v>
+      </c>
+      <c r="B136" s="8">
+        <v>5.2398999999999996</v>
+      </c>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="6"/>
+    </row>
+    <row r="137" spans="1:5" ht="17" customHeight="1">
+      <c r="A137" s="7">
+        <v>41426</v>
+      </c>
+      <c r="B137" s="8">
+        <v>5.3292000000000002</v>
+      </c>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+    </row>
+    <row r="138" spans="1:5" ht="17" customHeight="1">
+      <c r="A138" s="7">
+        <v>41456</v>
+      </c>
+      <c r="B138" s="8">
+        <v>5.4408772727272696</v>
+      </c>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+    </row>
+    <row r="139" spans="1:5" ht="17" customHeight="1">
+      <c r="A139" s="7">
+        <v>41487</v>
+      </c>
+      <c r="B139" s="8">
+        <v>5.5813666666666677</v>
+      </c>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+    </row>
+    <row r="140" spans="1:5" ht="17" customHeight="1">
+      <c r="A140" s="7">
+        <v>41518</v>
+      </c>
+      <c r="B140" s="8">
+        <v>5.7371238095238093</v>
+      </c>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+    </row>
+    <row r="141" spans="1:5" ht="17" customHeight="1">
+      <c r="A141" s="7">
+        <v>41548</v>
+      </c>
+      <c r="B141" s="8">
+        <v>5.8482000000000003</v>
+      </c>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+    </row>
+    <row r="142" spans="1:5" ht="17" customHeight="1">
+      <c r="A142" s="7">
+        <v>41579</v>
+      </c>
+      <c r="B142" s="8">
+        <v>6.0149368421052616</v>
+      </c>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+    </row>
+    <row r="143" spans="1:5" ht="17" customHeight="1">
+      <c r="A143" s="7">
+        <v>41609</v>
+      </c>
+      <c r="B143" s="8">
+        <v>6.3191789473684201</v>
+      </c>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+    </row>
+    <row r="144" spans="1:5" ht="17" customHeight="1">
+      <c r="A144" s="7">
+        <v>41640</v>
+      </c>
+      <c r="B144" s="8">
+        <v>7.0967272727272723</v>
+      </c>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="6"/>
+    </row>
+    <row r="145" spans="1:5" ht="17" customHeight="1">
+      <c r="A145" s="7">
+        <v>41671</v>
+      </c>
+      <c r="B145" s="8">
+        <v>7.8565299999999993</v>
+      </c>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+    </row>
+    <row r="146" spans="1:5" ht="17" customHeight="1">
+      <c r="A146" s="7">
+        <v>41700</v>
+      </c>
+      <c r="B146" s="9">
+        <v>7.9313000000000011</v>
+      </c>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+    </row>
+    <row r="147" spans="1:5" ht="17" customHeight="1">
+      <c r="A147" s="6"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV4422"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" workbookViewId="0">
+    <sheetView defaultGridColor="0" colorId="9" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -33960,1646 +35602,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV147"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="14.75" customHeight="1" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="8.125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.625" style="5" customWidth="1"/>
-    <col min="3" max="256" width="8.125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="17" customHeight="1">
-      <c r="A2" s="7">
-        <v>37316</v>
-      </c>
-      <c r="B2" s="8">
-        <v>2.398855555555556</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="17" customHeight="1">
-      <c r="A3" s="7">
-        <v>37347</v>
-      </c>
-      <c r="B3" s="8">
-        <v>2.8551062500000008</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1">
-      <c r="A4" s="7">
-        <v>37377</v>
-      </c>
-      <c r="B4" s="8">
-        <v>3.3287</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1">
-      <c r="A5" s="7">
-        <v>37408</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3.621300000000002</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1">
-      <c r="A6" s="7">
-        <v>37438</v>
-      </c>
-      <c r="B6" s="8">
-        <v>3.6071363636363638</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1">
-      <c r="A7" s="7">
-        <v>37469</v>
-      </c>
-      <c r="B7" s="8">
-        <v>3.6207095238095239</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1">
-      <c r="A8" s="7">
-        <v>37500</v>
-      </c>
-      <c r="B8" s="8">
-        <v>3.6430761904761901</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1">
-      <c r="A9" s="7">
-        <v>37530</v>
-      </c>
-      <c r="B9" s="8">
-        <v>3.6518818181818191</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1">
-      <c r="A10" s="7">
-        <v>37561</v>
-      </c>
-      <c r="B10" s="8">
-        <v>3.52555</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="17" customHeight="1">
-      <c r="A11" s="7">
-        <v>37591</v>
-      </c>
-      <c r="B11" s="8">
-        <v>3.4901714285714278</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="17" customHeight="1">
-      <c r="A12" s="7">
-        <v>37622</v>
-      </c>
-      <c r="B12" s="8">
-        <v>3.258186363636363</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="17" customHeight="1">
-      <c r="A13" s="7">
-        <v>37653</v>
-      </c>
-      <c r="B13" s="8">
-        <v>3.1631649999999989</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="17" customHeight="1">
-      <c r="A14" s="7">
-        <v>37681</v>
-      </c>
-      <c r="B14" s="8">
-        <v>3.0747249999999999</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="17" customHeight="1">
-      <c r="A15" s="7">
-        <v>37712</v>
-      </c>
-      <c r="B15" s="8">
-        <v>2.8946049999999999</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="17" customHeight="1">
-      <c r="A16" s="7">
-        <v>37742</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2.8356714285714291</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="17" customHeight="1">
-      <c r="A17" s="7">
-        <v>37773</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2.8088500000000001</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="17" customHeight="1">
-      <c r="A18" s="7">
-        <v>37803</v>
-      </c>
-      <c r="B18" s="8">
-        <v>2.801286363636363</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="17" customHeight="1">
-      <c r="A19" s="7">
-        <v>37834</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2.92849</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="17" customHeight="1">
-      <c r="A20" s="7">
-        <v>37865</v>
-      </c>
-      <c r="B20" s="8">
-        <v>2.9209454545454552</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="17" customHeight="1">
-      <c r="A21" s="7">
-        <v>37895</v>
-      </c>
-      <c r="B21" s="8">
-        <v>2.859049999999999</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="17" customHeight="1">
-      <c r="A22" s="7">
-        <v>37926</v>
-      </c>
-      <c r="B22" s="8">
-        <v>2.8839210526315791</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="17" customHeight="1">
-      <c r="A23" s="7">
-        <v>37956</v>
-      </c>
-      <c r="B23" s="8">
-        <v>2.9606238095238089</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="17" customHeight="1">
-      <c r="A24" s="7">
-        <v>37987</v>
-      </c>
-      <c r="B24" s="8">
-        <v>2.892842857142857</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="17" customHeight="1">
-      <c r="A25" s="7">
-        <v>38018</v>
-      </c>
-      <c r="B25" s="8">
-        <v>2.9319199999999999</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" ht="17" customHeight="1">
-      <c r="A26" s="7">
-        <v>38047</v>
-      </c>
-      <c r="B26" s="8">
-        <v>2.8975652173913051</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="17" customHeight="1">
-      <c r="A27" s="7">
-        <v>38078</v>
-      </c>
-      <c r="B27" s="8">
-        <v>2.8359157894736842</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" ht="17" customHeight="1">
-      <c r="A28" s="7">
-        <v>38108</v>
-      </c>
-      <c r="B28" s="8">
-        <v>2.9196750000000011</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="17" customHeight="1">
-      <c r="A29" s="7">
-        <v>38139</v>
-      </c>
-      <c r="B29" s="8">
-        <v>2.9602571428571429</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="17" customHeight="1">
-      <c r="A30" s="7">
-        <v>38169</v>
-      </c>
-      <c r="B30" s="8">
-        <v>2.9552142857142849</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="17" customHeight="1">
-      <c r="A31" s="7">
-        <v>38200</v>
-      </c>
-      <c r="B31" s="8">
-        <v>3.013580952380952</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" ht="17" customHeight="1">
-      <c r="A32" s="7">
-        <v>38231</v>
-      </c>
-      <c r="B32" s="8">
-        <v>2.996013636363636</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" ht="17" customHeight="1">
-      <c r="A33" s="7">
-        <v>38261</v>
-      </c>
-      <c r="B33" s="8">
-        <v>2.9691800000000002</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="17" customHeight="1">
-      <c r="A34" s="7">
-        <v>38292</v>
-      </c>
-      <c r="B34" s="8">
-        <v>2.9546363636363639</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" ht="17" customHeight="1">
-      <c r="A35" s="7">
-        <v>38322</v>
-      </c>
-      <c r="B35" s="8">
-        <v>2.970918181818182</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" ht="17" customHeight="1">
-      <c r="A36" s="7">
-        <v>38353</v>
-      </c>
-      <c r="B36" s="8">
-        <v>2.9460285714285721</v>
-      </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" ht="17" customHeight="1">
-      <c r="A37" s="7">
-        <v>38384</v>
-      </c>
-      <c r="B37" s="8">
-        <v>2.915344999999999</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" ht="17" customHeight="1">
-      <c r="A38" s="7">
-        <v>38412</v>
-      </c>
-      <c r="B38" s="8">
-        <v>2.9265523809523808</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" ht="17" customHeight="1">
-      <c r="A39" s="7">
-        <v>38443</v>
-      </c>
-      <c r="B39" s="8">
-        <v>2.9004142857142861</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" ht="17" customHeight="1">
-      <c r="A40" s="7">
-        <v>38473</v>
-      </c>
-      <c r="B40" s="8">
-        <v>2.89094761904762</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" ht="17" customHeight="1">
-      <c r="A41" s="7">
-        <v>38504</v>
-      </c>
-      <c r="B41" s="8">
-        <v>2.8835904761904758</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" ht="17" customHeight="1">
-      <c r="A42" s="7">
-        <v>38534</v>
-      </c>
-      <c r="B42" s="8">
-        <v>2.869566666666667</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" ht="17" customHeight="1">
-      <c r="A43" s="7">
-        <v>38565</v>
-      </c>
-      <c r="B43" s="8">
-        <v>2.888018181818182</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" ht="17" customHeight="1">
-      <c r="A44" s="7">
-        <v>38596</v>
-      </c>
-      <c r="B44" s="8">
-        <v>2.9117136363636358</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" ht="17" customHeight="1">
-      <c r="A45" s="7">
-        <v>38626</v>
-      </c>
-      <c r="B45" s="8">
-        <v>2.9660449999999998</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" ht="17" customHeight="1">
-      <c r="A46" s="7">
-        <v>38657</v>
-      </c>
-      <c r="B46" s="8">
-        <v>2.9672181818181809</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" ht="17" customHeight="1">
-      <c r="A47" s="7">
-        <v>38687</v>
-      </c>
-      <c r="B47" s="8">
-        <v>3.0144523809523811</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" ht="17" customHeight="1">
-      <c r="A48" s="7">
-        <v>38718</v>
-      </c>
-      <c r="B48" s="8">
-        <v>3.0460363636363641</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" ht="17" customHeight="1">
-      <c r="A49" s="7">
-        <v>38749</v>
-      </c>
-      <c r="B49" s="8">
-        <v>3.068905</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" ht="17" customHeight="1">
-      <c r="A50" s="7">
-        <v>38777</v>
-      </c>
-      <c r="B50" s="8">
-        <v>3.0763272727272728</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" ht="17" customHeight="1">
-      <c r="A51" s="7">
-        <v>38808</v>
-      </c>
-      <c r="B51" s="8">
-        <v>3.0662666666666669</v>
-      </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" ht="17" customHeight="1">
-      <c r="A52" s="7">
-        <v>38838</v>
-      </c>
-      <c r="B52" s="8">
-        <v>3.0534809523809519</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" ht="17" customHeight="1">
-      <c r="A53" s="7">
-        <v>38869</v>
-      </c>
-      <c r="B53" s="8">
-        <v>3.0812666666666662</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5" ht="17" customHeight="1">
-      <c r="A54" s="7">
-        <v>38899</v>
-      </c>
-      <c r="B54" s="8">
-        <v>3.0819619047619051</v>
-      </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:5" ht="17" customHeight="1">
-      <c r="A55" s="7">
-        <v>38930</v>
-      </c>
-      <c r="B55" s="8">
-        <v>3.0789727272727272</v>
-      </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-    </row>
-    <row r="56" spans="1:5" ht="17" customHeight="1">
-      <c r="A56" s="7">
-        <v>38961</v>
-      </c>
-      <c r="B56" s="8">
-        <v>3.1000714285714279</v>
-      </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:5" ht="17" customHeight="1">
-      <c r="A57" s="7">
-        <v>38991</v>
-      </c>
-      <c r="B57" s="8">
-        <v>3.0984761904761902</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="1:5" ht="17" customHeight="1">
-      <c r="A58" s="7">
-        <v>39022</v>
-      </c>
-      <c r="B58" s="8">
-        <v>3.075738095238095</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:5" ht="17" customHeight="1">
-      <c r="A59" s="7">
-        <v>39052</v>
-      </c>
-      <c r="B59" s="8">
-        <v>3.0602684210526312</v>
-      </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" spans="1:5" ht="17" customHeight="1">
-      <c r="A60" s="7">
-        <v>39083</v>
-      </c>
-      <c r="B60" s="8">
-        <v>3.085040909090909</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="1:5" ht="17" customHeight="1">
-      <c r="A61" s="7">
-        <v>39114</v>
-      </c>
-      <c r="B61" s="8">
-        <v>3.1026250000000002</v>
-      </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="1:5" ht="17" customHeight="1">
-      <c r="A62" s="7">
-        <v>39142</v>
-      </c>
-      <c r="B62" s="8">
-        <v>3.101040909090909</v>
-      </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" ht="17" customHeight="1">
-      <c r="A63" s="7">
-        <v>39173</v>
-      </c>
-      <c r="B63" s="8">
-        <v>3.089055555555555</v>
-      </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:5" ht="17" customHeight="1">
-      <c r="A64" s="7">
-        <v>39203</v>
-      </c>
-      <c r="B64" s="8">
-        <v>3.0800142857142871</v>
-      </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:5" ht="17" customHeight="1">
-      <c r="A65" s="7">
-        <v>39234</v>
-      </c>
-      <c r="B65" s="8">
-        <v>3.0792649999999999</v>
-      </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:5" ht="17" customHeight="1">
-      <c r="A66" s="7">
-        <v>39264</v>
-      </c>
-      <c r="B66" s="8">
-        <v>3.1116285714285721</v>
-      </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" ht="17" customHeight="1">
-      <c r="A67" s="7">
-        <v>39295</v>
-      </c>
-      <c r="B67" s="8">
-        <v>3.1523590909090902</v>
-      </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" ht="17" customHeight="1">
-      <c r="A68" s="7">
-        <v>39326</v>
-      </c>
-      <c r="B68" s="8">
-        <v>3.1474549999999999</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:5" ht="17" customHeight="1">
-      <c r="A69" s="7">
-        <v>39356</v>
-      </c>
-      <c r="B69" s="8">
-        <v>3.1604454545454539</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-    </row>
-    <row r="70" spans="1:5" ht="17" customHeight="1">
-      <c r="A70" s="7">
-        <v>39387</v>
-      </c>
-      <c r="B70" s="8">
-        <v>3.1359142857142861</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="1:5" ht="17" customHeight="1">
-      <c r="A71" s="7">
-        <v>39417</v>
-      </c>
-      <c r="B71" s="8">
-        <v>3.1396500000000001</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-    </row>
-    <row r="72" spans="1:5" ht="17" customHeight="1">
-      <c r="A72" s="7">
-        <v>39448</v>
-      </c>
-      <c r="B72" s="8">
-        <v>3.1444181818181818</v>
-      </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-    </row>
-    <row r="73" spans="1:5" ht="17" customHeight="1">
-      <c r="A73" s="7">
-        <v>39479</v>
-      </c>
-      <c r="B73" s="8">
-        <v>3.1583142857142859</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-    </row>
-    <row r="74" spans="1:5" ht="17" customHeight="1">
-      <c r="A74" s="7">
-        <v>39508</v>
-      </c>
-      <c r="B74" s="8">
-        <v>3.1558388888888889</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-    </row>
-    <row r="75" spans="1:5" ht="17" customHeight="1">
-      <c r="A75" s="7">
-        <v>39539</v>
-      </c>
-      <c r="B75" s="8">
-        <v>3.1665428571428582</v>
-      </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-    </row>
-    <row r="76" spans="1:5" ht="17" customHeight="1">
-      <c r="A76" s="7">
-        <v>39569</v>
-      </c>
-      <c r="B76" s="8">
-        <v>3.1511</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-    </row>
-    <row r="77" spans="1:5" ht="17" customHeight="1">
-      <c r="A77" s="7">
-        <v>39600</v>
-      </c>
-      <c r="B77" s="8">
-        <v>3.0433500000000011</v>
-      </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-    </row>
-    <row r="78" spans="1:5" ht="17" customHeight="1">
-      <c r="A78" s="7">
-        <v>39630</v>
-      </c>
-      <c r="B78" s="8">
-        <v>3.0223454545454551</v>
-      </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:5" ht="17" customHeight="1">
-      <c r="A79" s="7">
-        <v>39661</v>
-      </c>
-      <c r="B79" s="8">
-        <v>3.0332750000000002</v>
-      </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-    </row>
-    <row r="80" spans="1:5" ht="17" customHeight="1">
-      <c r="A80" s="7">
-        <v>39692</v>
-      </c>
-      <c r="B80" s="8">
-        <v>3.0823636363636369</v>
-      </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="1:5" ht="17" customHeight="1">
-      <c r="A81" s="7">
-        <v>39722</v>
-      </c>
-      <c r="B81" s="8">
-        <v>3.2385227272727271</v>
-      </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-    </row>
-    <row r="82" spans="1:5" ht="17" customHeight="1">
-      <c r="A82" s="7">
-        <v>39753</v>
-      </c>
-      <c r="B82" s="8">
-        <v>3.329173684210526</v>
-      </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-    </row>
-    <row r="83" spans="1:5" ht="17" customHeight="1">
-      <c r="A83" s="7">
-        <v>39783</v>
-      </c>
-      <c r="B83" s="8">
-        <v>3.4226333333333332</v>
-      </c>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-    </row>
-    <row r="84" spans="1:5" ht="17" customHeight="1">
-      <c r="A84" s="7">
-        <v>39814</v>
-      </c>
-      <c r="B84" s="8">
-        <v>3.4640142857142862</v>
-      </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-    </row>
-    <row r="85" spans="1:5" ht="17" customHeight="1">
-      <c r="A85" s="7">
-        <v>39845</v>
-      </c>
-      <c r="B85" s="8">
-        <v>3.5115149999999988</v>
-      </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-    </row>
-    <row r="86" spans="1:5" ht="17" customHeight="1">
-      <c r="A86" s="7">
-        <v>39873</v>
-      </c>
-      <c r="B86" s="8">
-        <v>3.6539714285714289</v>
-      </c>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-    </row>
-    <row r="87" spans="1:5" ht="17" customHeight="1">
-      <c r="A87" s="7">
-        <v>39904</v>
-      </c>
-      <c r="B87" s="8">
-        <v>3.6933736842105271</v>
-      </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-    </row>
-    <row r="88" spans="1:5" ht="17" customHeight="1">
-      <c r="A88" s="7">
-        <v>39934</v>
-      </c>
-      <c r="B88" s="8">
-        <v>3.7244736842105262</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-    </row>
-    <row r="89" spans="1:5" ht="17" customHeight="1">
-      <c r="A89" s="7">
-        <v>39965</v>
-      </c>
-      <c r="B89" s="8">
-        <v>3.7681333333333331</v>
-      </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
-    </row>
-    <row r="90" spans="1:5" ht="17" customHeight="1">
-      <c r="A90" s="7">
-        <v>39995</v>
-      </c>
-      <c r="B90" s="8">
-        <v>3.809733333333333</v>
-      </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
-    </row>
-    <row r="91" spans="1:5" ht="17" customHeight="1">
-      <c r="A91" s="7">
-        <v>40026</v>
-      </c>
-      <c r="B91" s="8">
-        <v>3.839175</v>
-      </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
-    </row>
-    <row r="92" spans="1:5" ht="17" customHeight="1">
-      <c r="A92" s="7">
-        <v>40057</v>
-      </c>
-      <c r="B92" s="8">
-        <v>3.842368181818181</v>
-      </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
-    </row>
-    <row r="93" spans="1:5" ht="17" customHeight="1">
-      <c r="A93" s="7">
-        <v>40087</v>
-      </c>
-      <c r="B93" s="8">
-        <v>3.8262095238095242</v>
-      </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
-    </row>
-    <row r="94" spans="1:5" ht="17" customHeight="1">
-      <c r="A94" s="7">
-        <v>40118</v>
-      </c>
-      <c r="B94" s="8">
-        <v>3.8109500000000001</v>
-      </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
-    </row>
-    <row r="95" spans="1:5" ht="17" customHeight="1">
-      <c r="A95" s="7">
-        <v>40148</v>
-      </c>
-      <c r="B95" s="8">
-        <v>3.8070190476190482</v>
-      </c>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
-    </row>
-    <row r="96" spans="1:5" ht="17" customHeight="1">
-      <c r="A96" s="7">
-        <v>40179</v>
-      </c>
-      <c r="B96" s="8">
-        <v>3.80416</v>
-      </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-    </row>
-    <row r="97" spans="1:5" ht="17" customHeight="1">
-      <c r="A97" s="7">
-        <v>40210</v>
-      </c>
-      <c r="B97" s="8">
-        <v>3.851235</v>
-      </c>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-    </row>
-    <row r="98" spans="1:5" ht="17" customHeight="1">
-      <c r="A98" s="7">
-        <v>40238</v>
-      </c>
-      <c r="B98" s="8">
-        <v>3.8627409090909088</v>
-      </c>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
-    </row>
-    <row r="99" spans="1:5" ht="17" customHeight="1">
-      <c r="A99" s="7">
-        <v>40269</v>
-      </c>
-      <c r="B99" s="8">
-        <v>3.8760699999999999</v>
-      </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
-    </row>
-    <row r="100" spans="1:5" ht="17" customHeight="1">
-      <c r="A100" s="7">
-        <v>40299</v>
-      </c>
-      <c r="B100" s="8">
-        <v>3.9019736842105259</v>
-      </c>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-    </row>
-    <row r="101" spans="1:5" ht="17" customHeight="1">
-      <c r="A101" s="7">
-        <v>40330</v>
-      </c>
-      <c r="B101" s="8">
-        <v>3.9265238095238102</v>
-      </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-    </row>
-    <row r="102" spans="1:5" ht="17" customHeight="1">
-      <c r="A102" s="7">
-        <v>40360</v>
-      </c>
-      <c r="B102" s="8">
-        <v>3.9348238095238099</v>
-      </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-    </row>
-    <row r="103" spans="1:5" ht="17" customHeight="1">
-      <c r="A103" s="7">
-        <v>40391</v>
-      </c>
-      <c r="B103" s="8">
-        <v>3.937609523809523</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-    </row>
-    <row r="104" spans="1:5" ht="17" customHeight="1">
-      <c r="A104" s="7">
-        <v>40422</v>
-      </c>
-      <c r="B104" s="8">
-        <v>3.9518909090909098</v>
-      </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-    </row>
-    <row r="105" spans="1:5" ht="17" customHeight="1">
-      <c r="A105" s="7">
-        <v>40452</v>
-      </c>
-      <c r="B105" s="8">
-        <v>3.9569999999999999</v>
-      </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-    </row>
-    <row r="106" spans="1:5" ht="17" customHeight="1">
-      <c r="A106" s="7">
-        <v>40483</v>
-      </c>
-      <c r="B106" s="8">
-        <v>3.9676</v>
-      </c>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-    </row>
-    <row r="107" spans="1:5" ht="17" customHeight="1">
-      <c r="A107" s="7">
-        <v>40513</v>
-      </c>
-      <c r="B107" s="8">
-        <v>3.9776250000000002</v>
-      </c>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="6"/>
-    </row>
-    <row r="108" spans="1:5" ht="17" customHeight="1">
-      <c r="A108" s="7">
-        <v>40544</v>
-      </c>
-      <c r="B108" s="8">
-        <v>3.9813000000000001</v>
-      </c>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
-    </row>
-    <row r="109" spans="1:5" ht="17" customHeight="1">
-      <c r="A109" s="7">
-        <v>40575</v>
-      </c>
-      <c r="B109" s="8">
-        <v>4.0220000000000002</v>
-      </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-    </row>
-    <row r="110" spans="1:5" ht="17" customHeight="1">
-      <c r="A110" s="7">
-        <v>40603</v>
-      </c>
-      <c r="B110" s="8">
-        <v>4.0372000000000003</v>
-      </c>
-      <c r="C110" s="6"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="6"/>
-    </row>
-    <row r="111" spans="1:5" ht="17" customHeight="1">
-      <c r="A111" s="7">
-        <v>40634</v>
-      </c>
-      <c r="B111" s="8">
-        <v>4.0655000000000001</v>
-      </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
-    </row>
-    <row r="112" spans="1:5" ht="17" customHeight="1">
-      <c r="A112" s="7">
-        <v>40664</v>
-      </c>
-      <c r="B112" s="8">
-        <v>4.0838999999999999</v>
-      </c>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6"/>
-    </row>
-    <row r="113" spans="1:5" ht="17" customHeight="1">
-      <c r="A113" s="7">
-        <v>40695</v>
-      </c>
-      <c r="B113" s="8">
-        <v>4.0960000000000001</v>
-      </c>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
-    </row>
-    <row r="114" spans="1:5" ht="17" customHeight="1">
-      <c r="A114" s="7">
-        <v>40725</v>
-      </c>
-      <c r="B114" s="8">
-        <v>4.1276000000000002</v>
-      </c>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
-    </row>
-    <row r="115" spans="1:5" ht="17" customHeight="1">
-      <c r="A115" s="7">
-        <v>40756</v>
-      </c>
-      <c r="B115" s="8">
-        <v>4.1680000000000001</v>
-      </c>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
-    </row>
-    <row r="116" spans="1:5" ht="17" customHeight="1">
-      <c r="A116" s="7">
-        <v>40787</v>
-      </c>
-      <c r="B116" s="8">
-        <v>4.2042000000000002</v>
-      </c>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
-    </row>
-    <row r="117" spans="1:5" ht="17" customHeight="1">
-      <c r="A117" s="7">
-        <v>40817</v>
-      </c>
-      <c r="B117" s="8">
-        <v>4.2221249999999992</v>
-      </c>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
-    </row>
-    <row r="118" spans="1:5" ht="17" customHeight="1">
-      <c r="A118" s="7">
-        <v>40848</v>
-      </c>
-      <c r="B118" s="8">
-        <v>4.2601142857142849</v>
-      </c>
-      <c r="C118" s="6"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="6"/>
-    </row>
-    <row r="119" spans="1:5" ht="17" customHeight="1">
-      <c r="A119" s="7">
-        <v>40878</v>
-      </c>
-      <c r="B119" s="8">
-        <v>4.2887894736842096</v>
-      </c>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
-    </row>
-    <row r="120" spans="1:5" ht="17" customHeight="1">
-      <c r="A120" s="7">
-        <v>40909</v>
-      </c>
-      <c r="B120" s="8">
-        <v>4.3206238095238101</v>
-      </c>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-    </row>
-    <row r="121" spans="1:5" ht="17" customHeight="1">
-      <c r="A121" s="7">
-        <v>40940</v>
-      </c>
-      <c r="B121" s="8">
-        <v>4.3462944444444442</v>
-      </c>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-    </row>
-    <row r="122" spans="1:5" ht="17" customHeight="1">
-      <c r="A122" s="7">
-        <v>40969</v>
-      </c>
-      <c r="B122" s="8">
-        <v>4.3563136363636357</v>
-      </c>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-    </row>
-    <row r="123" spans="1:5" ht="17" customHeight="1">
-      <c r="A123" s="7">
-        <v>41000</v>
-      </c>
-      <c r="B123" s="8">
-        <v>4.3978000000000002</v>
-      </c>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="6"/>
-    </row>
-    <row r="124" spans="1:5" ht="17" customHeight="1">
-      <c r="A124" s="7">
-        <v>41030</v>
-      </c>
-      <c r="B124" s="8">
-        <v>4.4503761904761907</v>
-      </c>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="6"/>
-    </row>
-    <row r="125" spans="1:5" ht="17" customHeight="1">
-      <c r="A125" s="7">
-        <v>41061</v>
-      </c>
-      <c r="B125" s="8">
-        <v>4.4977549999999997</v>
-      </c>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
-      <c r="E125" s="6"/>
-    </row>
-    <row r="126" spans="1:5" ht="17" customHeight="1">
-      <c r="A126" s="7">
-        <v>41091</v>
-      </c>
-      <c r="B126" s="8">
-        <v>4.5528095238095254</v>
-      </c>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-    </row>
-    <row r="127" spans="1:5" ht="17" customHeight="1">
-      <c r="A127" s="7">
-        <v>41122</v>
-      </c>
-      <c r="B127" s="8">
-        <v>4.6098272727272729</v>
-      </c>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="6"/>
-    </row>
-    <row r="128" spans="1:5" ht="17" customHeight="1">
-      <c r="A128" s="7">
-        <v>41153</v>
-      </c>
-      <c r="B128" s="8">
-        <v>4.6698947368421049</v>
-      </c>
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="6"/>
-    </row>
-    <row r="129" spans="1:5" ht="17" customHeight="1">
-      <c r="A129" s="7">
-        <v>41183</v>
-      </c>
-      <c r="B129" s="8">
-        <v>4.7298500000000008</v>
-      </c>
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
-    </row>
-    <row r="130" spans="1:5" ht="17" customHeight="1">
-      <c r="A130" s="7">
-        <v>41214</v>
-      </c>
-      <c r="B130" s="8">
-        <v>4.7973899999999992</v>
-      </c>
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-    </row>
-    <row r="131" spans="1:5" ht="17" customHeight="1">
-      <c r="A131" s="7">
-        <v>41244</v>
-      </c>
-      <c r="B131" s="8">
-        <v>4.88</v>
-      </c>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="6"/>
-    </row>
-    <row r="132" spans="1:5" ht="17" customHeight="1">
-      <c r="A132" s="7">
-        <v>41275</v>
-      </c>
-      <c r="B132" s="8">
-        <v>4.9485999999999999</v>
-      </c>
-      <c r="C132" s="6"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="6"/>
-    </row>
-    <row r="133" spans="1:5" ht="17" customHeight="1">
-      <c r="A133" s="7">
-        <v>41306</v>
-      </c>
-      <c r="B133" s="8">
-        <v>5.0110999999999999</v>
-      </c>
-      <c r="C133" s="6"/>
-      <c r="D133" s="6"/>
-      <c r="E133" s="6"/>
-    </row>
-    <row r="134" spans="1:5" ht="17" customHeight="1">
-      <c r="A134" s="7">
-        <v>41334</v>
-      </c>
-      <c r="B134" s="8">
-        <v>5.0839999999999996</v>
-      </c>
-      <c r="C134" s="6"/>
-      <c r="D134" s="6"/>
-      <c r="E134" s="6"/>
-    </row>
-    <row r="135" spans="1:5" ht="17" customHeight="1">
-      <c r="A135" s="7">
-        <v>41365</v>
-      </c>
-      <c r="B135" s="8">
-        <v>5.1555</v>
-      </c>
-      <c r="C135" s="6"/>
-      <c r="D135" s="6"/>
-      <c r="E135" s="6"/>
-    </row>
-    <row r="136" spans="1:5" ht="17" customHeight="1">
-      <c r="A136" s="7">
-        <v>41395</v>
-      </c>
-      <c r="B136" s="8">
-        <v>5.2398999999999996</v>
-      </c>
-      <c r="C136" s="6"/>
-      <c r="D136" s="6"/>
-      <c r="E136" s="6"/>
-    </row>
-    <row r="137" spans="1:5" ht="17" customHeight="1">
-      <c r="A137" s="7">
-        <v>41426</v>
-      </c>
-      <c r="B137" s="8">
-        <v>5.3292000000000002</v>
-      </c>
-      <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
-      <c r="E137" s="6"/>
-    </row>
-    <row r="138" spans="1:5" ht="17" customHeight="1">
-      <c r="A138" s="7">
-        <v>41456</v>
-      </c>
-      <c r="B138" s="8">
-        <v>5.4408772727272696</v>
-      </c>
-      <c r="C138" s="6"/>
-      <c r="D138" s="6"/>
-      <c r="E138" s="6"/>
-    </row>
-    <row r="139" spans="1:5" ht="17" customHeight="1">
-      <c r="A139" s="7">
-        <v>41487</v>
-      </c>
-      <c r="B139" s="8">
-        <v>5.5813666666666677</v>
-      </c>
-      <c r="C139" s="6"/>
-      <c r="D139" s="6"/>
-      <c r="E139" s="6"/>
-    </row>
-    <row r="140" spans="1:5" ht="17" customHeight="1">
-      <c r="A140" s="7">
-        <v>41518</v>
-      </c>
-      <c r="B140" s="8">
-        <v>5.7371238095238093</v>
-      </c>
-      <c r="C140" s="6"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="6"/>
-    </row>
-    <row r="141" spans="1:5" ht="17" customHeight="1">
-      <c r="A141" s="7">
-        <v>41548</v>
-      </c>
-      <c r="B141" s="8">
-        <v>5.8482000000000003</v>
-      </c>
-      <c r="C141" s="6"/>
-      <c r="D141" s="6"/>
-      <c r="E141" s="6"/>
-    </row>
-    <row r="142" spans="1:5" ht="17" customHeight="1">
-      <c r="A142" s="7">
-        <v>41579</v>
-      </c>
-      <c r="B142" s="8">
-        <v>6.0149368421052616</v>
-      </c>
-      <c r="C142" s="6"/>
-      <c r="D142" s="6"/>
-      <c r="E142" s="6"/>
-    </row>
-    <row r="143" spans="1:5" ht="17" customHeight="1">
-      <c r="A143" s="7">
-        <v>41609</v>
-      </c>
-      <c r="B143" s="8">
-        <v>6.3191789473684201</v>
-      </c>
-      <c r="C143" s="6"/>
-      <c r="D143" s="6"/>
-      <c r="E143" s="6"/>
-    </row>
-    <row r="144" spans="1:5" ht="17" customHeight="1">
-      <c r="A144" s="7">
-        <v>41640</v>
-      </c>
-      <c r="B144" s="8">
-        <v>7.0967272727272723</v>
-      </c>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6"/>
-    </row>
-    <row r="145" spans="1:5" ht="17" customHeight="1">
-      <c r="A145" s="7">
-        <v>41671</v>
-      </c>
-      <c r="B145" s="8">
-        <v>7.8565299999999993</v>
-      </c>
-      <c r="C145" s="6"/>
-      <c r="D145" s="6"/>
-      <c r="E145" s="6"/>
-    </row>
-    <row r="146" spans="1:5" ht="17" customHeight="1">
-      <c r="A146" s="7">
-        <v>41700</v>
-      </c>
-      <c r="B146" s="9">
-        <v>7.9313000000000011</v>
-      </c>
-      <c r="C146" s="6"/>
-      <c r="D146" s="6"/>
-      <c r="E146" s="6"/>
-    </row>
-    <row r="147" spans="1:5" ht="17" customHeight="1">
-      <c r="A147" s="6"/>
-      <c r="B147" s="10"/>
-      <c r="C147" s="6"/>
-      <c r="D147" s="6"/>
-      <c r="E147" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>